<commit_message>
list of properties and classes
</commit_message>
<xml_diff>
--- a/inst/classes_and_properties.xlsx
+++ b/inst/classes_and_properties.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="V1-2" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V1-2'!$A$3:$G$36</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -146,9 +149,6 @@
     <t>dct:conformsTo</t>
   </si>
   <si>
-    <t>M (replaced by dct:license)</t>
-  </si>
-  <si>
     <t>dct:byteSize</t>
   </si>
   <si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>dcat:temporalResolution</t>
+  </si>
+  <si>
+    <t>M (replaced by dct:license, now O)</t>
   </si>
 </sst>
 </file>
@@ -483,16 +486,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" customWidth="1"/>
-    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -545,7 +554,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -556,7 +565,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -567,7 +576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -598,7 +607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -612,7 +621,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -626,7 +635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -645,7 +654,7 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -674,7 +683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -682,7 +691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -696,7 +705,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -704,7 +713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -718,7 +727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -746,7 +755,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -757,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -768,7 +777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -779,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -820,7 +829,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -831,7 +840,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -839,7 +848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -847,7 +856,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -855,7 +864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -866,7 +875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -874,39 +883,46 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D36" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:G36">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add filters to columns
</commit_message>
<xml_diff>
--- a/inst/classes_and_properties.xlsx
+++ b/inst/classes_and_properties.xlsx
@@ -486,11 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -554,7 +553,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -565,7 +564,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -576,7 +575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -607,7 +606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -621,7 +620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -635,7 +634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -683,7 +682,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -691,7 +690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -705,7 +704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -713,7 +712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -727,7 +726,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -755,7 +754,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -766,7 +765,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -777,7 +776,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -788,7 +787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -829,7 +828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -840,7 +839,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -848,7 +847,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -856,7 +855,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -864,7 +863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -875,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -883,7 +882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -891,7 +890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -899,7 +898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -907,7 +906,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -916,13 +915,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G36">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:G36"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set print area (all on one page) and borders
</commit_message>
<xml_diff>
--- a/inst/classes_and_properties.xlsx
+++ b/inst/classes_and_properties.xlsx
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V1-2'!$A$3:$G$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'V1-2'!$A$1:$G$36</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -168,9 +169,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -191,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -199,14 +207,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -489,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,425 +529,565 @@
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
-        <v>30</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
-        <v>30</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" t="s">
-        <v>30</v>
-      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" t="s">
-        <v>30</v>
-      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" t="s">
-        <v>30</v>
-      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G25" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" t="s">
-        <v>32</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D36" t="s">
-        <v>32</v>
-      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:G36"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>